<commit_message>
added desctools to calculate CCC
</commit_message>
<xml_diff>
--- a/R_files_final/patient_data.xlsx
+++ b/R_files_final/patient_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tegin/Desktop/GitHub2/SARS-CoV-2_in_housepets/R_files_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8258AC5-AB50-EF4D-BFE2-887793358F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A07ED7-3A7E-D445-BA13-8E4DA8EE99E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - C__Users_tegin_Deskto" sheetId="1" r:id="rId1"/>
@@ -662,10 +662,10 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -674,19 +674,19 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -707,22 +707,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1891,10 +1891,10 @@
   <dimension ref="A1:AT65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="V19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ7" sqref="AQ7"/>
+      <selection pane="bottomRight" activeCell="AG38" sqref="AG38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5524,10 +5524,10 @@
         <v>0</v>
       </c>
       <c r="Z26" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA26" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB26" s="8">
         <v>0</v>
@@ -5560,7 +5560,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM26" s="8">
         <v>0</v>
@@ -6084,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="Z30" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA30" s="18">
         <v>0</v>
@@ -6111,7 +6111,7 @@
         <v>0</v>
       </c>
       <c r="AI30" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ30" s="8">
         <v>0</v>
@@ -6224,7 +6224,7 @@
         <v>31</v>
       </c>
       <c r="Z31" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA31" s="18">
         <v>0</v>
@@ -6245,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="AG31" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="8">
         <v>0</v>
@@ -7204,25 +7204,25 @@
         <v>1</v>
       </c>
       <c r="Z38" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA38" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB38" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="8">
         <v>0</v>
       </c>
       <c r="AD38" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE38" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG38" s="8">
         <v>0</v>

</xml_diff>